<commit_message>
Add Excel-style filtering with live search to Database Library Manager
- Added Excel-style column header filtering to Tables and Fields ListViews
- Implemented live search textbox in filter windows for instant filtering
- Added cumulative filtering support (filters work together like Excel)
- Filter states preserved across search operations
- Enhanced FilterWindowContentForm with search capabilities
- Added JoinControl for query builder functionality
- Updated database models and services
</commit_message>
<xml_diff>
--- a/Features to add.xlsx
+++ b/Features to add.xlsx
@@ -2,19 +2,20 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
-  <workbookPr defaultThemeVersion="202300"/>
+  <workbookPr codeName="ThisWorkbook" defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ab7y02\OneDrive - American National Insurance Company\Documents\Code Projects\C#\CSuiteView\CSuiteView\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://anico-my.sharepoint.com/personal/ab7y02_dnanico1_aniconet_com/Documents/Documents/Code Projects/C#/CSuiteView/CSuiteView/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1CF8693B-47DC-4430-9559-FF6091CBD4AE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="50" documentId="13_ncr:1_{1CF8693B-47DC-4430-9559-FF6091CBD4AE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A3D8F9D3-045D-4482-8674-FA3DC85B81DE}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{CF1343FB-A9C9-4CCE-8FF6-D066FE804AF7}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$O$2</definedName>
@@ -40,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="68">
   <si>
     <t>Phs</t>
   </si>
@@ -216,17 +217,41 @@
     <t>Run the query and display results</t>
   </si>
   <si>
-    <t xml:space="preserve">At the top of the form for the query should be a button called "Run".  When this button is clicked the SQL string should be build accordign to whats in the Criteria, Display and Tables tab.  The sql string then be formated and printed to the SQL tab.  The results of the query should be put into the Results sheet.  </t>
-  </si>
-  <si>
     <t>This is important, the results could be quite large, like 1,000,000 rows or more is possible.  Check the size of the output to determine how to display the results.  If the results are quite large you may need to use code that will be much more permant in viewing the data.  If the results are smaller, like 20,000, we can use a display method that isnt as complicated.</t>
+  </si>
+  <si>
+    <t>Click on Company_Data to add a data source</t>
+  </si>
+  <si>
+    <t>When you click on company data, the middel workspace should show a input box with a label that says Name your Company_Data.   Another input box with a label below it that says ODBC datasource name.  And a button that says Add</t>
+  </si>
+  <si>
+    <t>When you click on the button, the name is added as a child under Company_Data. And the Data Source is queried to show all the tables just like we have for UL_Rates</t>
+  </si>
+  <si>
+    <t>Complete</t>
+  </si>
+  <si>
+    <t>I no longer want to click on the tree node of "Company_Data" to add new data sources.  Instead next to Data Sources label I want a small brass button that says "Add", and have it wired to the same page of inputs that used to be for Company_Data click</t>
+  </si>
+  <si>
+    <t>And do the same for My Queries - add a small brass button that "Add" and use that for the add functionality</t>
+  </si>
+  <si>
+    <t>I want the Edit ability disabled by default. then add an "Edit" button that is in that secondary light blue color, add it under the Data Sources list box.  When this button is clicked I wanto enable the delete functionality.  Also when that button is click I want in big red letters in the bottom middle "EDIT MODE ON.  OBEJCTS CAN BE DELETED".  And i want the edit button to now say Disable in red text.  When th eDisable button i click, the red text goes away, you cannot right click to delete objects and the button goes back to saying Edit and the color goes back as well.</t>
+  </si>
+  <si>
+    <t>When clickign on a data source like Life_Prod, I want the add button to be above the table data in the middle. Move the table down a bit and add the button and make is be brass colored.  See image</t>
+  </si>
+  <si>
+    <t xml:space="preserve">When i select a query, at the top of the form for the query should be a button called "Run".  When this button is clicked the SQL string should be built accordin gto whats in the Criteria, Display and Tables tab.  The sql string then be formated and printed to the SQL tab.  The results of the query should be put into the Results sheet.  </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -248,13 +273,25 @@
       <name val="Segoe UI"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="10">
@@ -358,7 +395,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -388,6 +425,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="2"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -403,6 +441,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -722,6 +764,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{47E55E30-E45C-40CC-A26B-2630D6710CCF}">
+  <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:O25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -983,7 +1026,8 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{66F658BC-4370-4E5F-B120-93FCBC02230D}">
-  <dimension ref="C2:D38"/>
+  <sheetPr codeName="Sheet2"/>
+  <dimension ref="B2:D55"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
       <selection activeCell="C38" sqref="C38"/>
@@ -991,64 +1035,68 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="2" max="2" width="11.140625" customWidth="1"/>
     <col min="3" max="3" width="26.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B2" s="19" t="s">
+        <v>62</v>
+      </c>
       <c r="C2" s="15" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="3" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:4" x14ac:dyDescent="0.25">
       <c r="C3" s="16" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="4" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:4" x14ac:dyDescent="0.25">
       <c r="C4" s="16" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="5" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:4" x14ac:dyDescent="0.25">
       <c r="C5" s="18" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="6" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:4" x14ac:dyDescent="0.25">
       <c r="C6" s="18" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="7" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:4" x14ac:dyDescent="0.25">
       <c r="C7" s="18" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="8" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:4" x14ac:dyDescent="0.25">
       <c r="C8" s="17"/>
     </row>
-    <row r="9" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:4" x14ac:dyDescent="0.25">
       <c r="C9" s="15" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="10" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:4" x14ac:dyDescent="0.25">
       <c r="C10" s="17" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="11" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:4" x14ac:dyDescent="0.25">
       <c r="C11" s="14"/>
     </row>
-    <row r="12" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:4" x14ac:dyDescent="0.25">
       <c r="C12" s="14"/>
     </row>
-    <row r="13" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:4" x14ac:dyDescent="0.25">
       <c r="C13" s="15" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="14" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:4" x14ac:dyDescent="0.25">
       <c r="C14" s="16" t="s">
         <v>42</v>
       </c>
@@ -1056,7 +1104,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="15" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:4" x14ac:dyDescent="0.25">
       <c r="C15" s="16" t="s">
         <v>44</v>
       </c>
@@ -1064,86 +1112,164 @@
         <v>45</v>
       </c>
     </row>
-    <row r="16" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:4" x14ac:dyDescent="0.25">
       <c r="C16" s="16"/>
     </row>
-    <row r="17" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C17" s="15" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="18" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C18" s="17" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="23" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B23" s="19" t="s">
+        <v>62</v>
+      </c>
       <c r="C23" s="15" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="24" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C24" s="16" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="25" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C25" s="16"/>
     </row>
-    <row r="26" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C26" s="15" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="27" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C27" s="16" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="28" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C28" s="16" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="29" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C29" s="16" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="30" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C30" s="16" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="33" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C33" s="15" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="34" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C34" s="16" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="35" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C35" s="16"/>
     </row>
-    <row r="36" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C36" s="15" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="37" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C37" s="16" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="38" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C38" s="16" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="38" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C38" s="16" t="s">
+    <row r="42" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B42" s="19" t="s">
+        <v>62</v>
+      </c>
+      <c r="C42" s="15" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="43" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C43" s="16" t="s">
         <v>59</v>
+      </c>
+    </row>
+    <row r="44" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C44" s="16"/>
+    </row>
+    <row r="45" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C45" s="15" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="46" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C46" s="16" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="47" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C47" s="16" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="50" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B50" s="19" t="s">
+        <v>62</v>
+      </c>
+      <c r="C50" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="51" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C51" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="53" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B53" s="19" t="s">
+        <v>62</v>
+      </c>
+      <c r="C53" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="55" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B55" s="19" t="s">
+        <v>62</v>
+      </c>
+      <c r="C55" t="s">
+        <v>66</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{84D284D5-C108-42B3-8031-02B39DE8D157}">
+  <sheetPr codeName="Sheet3"/>
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H6" sqref="H6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>